<commit_message>
lab 4 и lab 5
</commit_message>
<xml_diff>
--- a/PASKurs/лабораторные работы/l2/PAS2.PAS1.xlsx
+++ b/PASKurs/лабораторные работы/l2/PAS2.PAS1.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work\KursPro\PASKurs\лабораторные работы\l2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work\GitHub projects\KursPro\PASKurs\лабораторные работы\l2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC570D1-8D95-440E-9B66-FB845823A856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="375" windowWidth="14445" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="96" yWindow="372" windowWidth="14448" windowHeight="11388" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PAS2 - TODO" sheetId="6" r:id="rId1"/>
@@ -20,7 +19,7 @@
     <sheet name="5-РКПСиОК" sheetId="1" state="hidden" r:id="rId5"/>
     <sheet name="6-РКИСиРК" sheetId="4" state="hidden" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="131">
   <si>
     <t>З1</t>
   </si>
@@ -429,12 +428,15 @@
   </si>
   <si>
     <t>23 - 25</t>
+  </si>
+  <si>
+    <t>Сервер</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2083,6 +2085,123 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="80" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="75" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="78" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="92" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="93" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="71" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="69" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="91" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="94" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="95" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="96" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2098,12 +2217,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="91" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="94" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2122,9 +2235,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2139,114 +2249,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="92" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="93" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="71" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="69" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="94" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="95" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="96" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="80" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="75" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="78" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2579,21 +2581,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0404A7BF-071F-4896-BE14-9724EED32E76}">
-  <dimension ref="C3:E9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31:C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C3" s="81" t="s">
         <v>121</v>
       </c>
@@ -2604,7 +2606,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C4" s="81" t="s">
         <v>5</v>
       </c>
@@ -2615,7 +2617,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C5" s="81" t="s">
         <v>6</v>
       </c>
@@ -2626,7 +2628,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C6" s="81" t="s">
         <v>7</v>
       </c>
@@ -2637,7 +2639,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C7" s="81" t="s">
         <v>8</v>
       </c>
@@ -2648,7 +2650,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C8" s="81" t="s">
         <v>9</v>
       </c>
@@ -2659,7 +2661,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C9" s="81" t="s">
         <v>110</v>
       </c>
@@ -2668,6 +2670,28 @@
       </c>
       <c r="E9" s="81">
         <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C10" s="81" t="s">
+        <v>130</v>
+      </c>
+      <c r="D10" s="81">
+        <v>1</v>
+      </c>
+      <c r="E10" s="81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C11" s="81"/>
+      <c r="D11" s="81">
+        <f>SUM(D4:D10)</f>
+        <v>27</v>
+      </c>
+      <c r="E11" s="81">
+        <f>SUM(E4:E10)</f>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -2676,56 +2700,56 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" customWidth="1"/>
-    <col min="14" max="14" width="10.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" customWidth="1"/>
+    <col min="9" max="9" width="13.88671875" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" customWidth="1"/>
+    <col min="12" max="12" width="10.88671875" customWidth="1"/>
+    <col min="14" max="14" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="146" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" s="142" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="172" t="s">
+      <c r="B1" s="133" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="173"/>
-      <c r="D1" s="174"/>
-      <c r="E1" s="166" t="s">
+      <c r="C1" s="134"/>
+      <c r="D1" s="135"/>
+      <c r="E1" s="127" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="167"/>
-      <c r="G1" s="167"/>
-      <c r="H1" s="167"/>
-      <c r="I1" s="167"/>
-      <c r="J1" s="168"/>
-      <c r="K1" s="162" t="s">
+      <c r="F1" s="128"/>
+      <c r="G1" s="128"/>
+      <c r="H1" s="128"/>
+      <c r="I1" s="128"/>
+      <c r="J1" s="129"/>
+      <c r="K1" s="123" t="s">
         <v>59</v>
       </c>
-      <c r="L1" s="164" t="s">
+      <c r="L1" s="125" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="146"/>
-      <c r="B2" s="172"/>
-      <c r="C2" s="173"/>
-      <c r="D2" s="174"/>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" s="142"/>
+      <c r="B2" s="133"/>
+      <c r="C2" s="134"/>
+      <c r="D2" s="135"/>
       <c r="E2" s="69" t="s">
         <v>5</v>
       </c>
@@ -2744,31 +2768,31 @@
       <c r="J2" s="70" t="s">
         <v>110</v>
       </c>
-      <c r="K2" s="162"/>
-      <c r="L2" s="164"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="146"/>
-      <c r="B3" s="172"/>
-      <c r="C3" s="173"/>
-      <c r="D3" s="174"/>
-      <c r="E3" s="169" t="s">
+      <c r="K2" s="123"/>
+      <c r="L2" s="125"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="142"/>
+      <c r="B3" s="133"/>
+      <c r="C3" s="134"/>
+      <c r="D3" s="135"/>
+      <c r="E3" s="130" t="s">
         <v>104</v>
       </c>
-      <c r="F3" s="170"/>
-      <c r="G3" s="170"/>
-      <c r="H3" s="170"/>
-      <c r="I3" s="170"/>
-      <c r="J3" s="171"/>
-      <c r="K3" s="163"/>
-      <c r="L3" s="165"/>
+      <c r="F3" s="131"/>
+      <c r="G3" s="131"/>
+      <c r="H3" s="131"/>
+      <c r="I3" s="131"/>
+      <c r="J3" s="132"/>
+      <c r="K3" s="124"/>
+      <c r="L3" s="126"/>
       <c r="O3" s="84"/>
     </row>
-    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="147"/>
-      <c r="B4" s="175"/>
-      <c r="C4" s="176"/>
-      <c r="D4" s="177"/>
+    <row r="4" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="143"/>
+      <c r="B4" s="136"/>
+      <c r="C4" s="137"/>
+      <c r="D4" s="138"/>
       <c r="E4" s="75" t="str">
         <f>'4-ОМК'!I7</f>
         <v>1 -  11</v>
@@ -2802,7 +2826,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="14.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="14.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A5" s="46">
         <v>1</v>
       </c>
@@ -2836,15 +2860,15 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="86">
         <v>2</v>
       </c>
-      <c r="B6" s="148" t="s">
+      <c r="B6" s="144" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="149"/>
-      <c r="D6" s="150"/>
+      <c r="C6" s="145"/>
+      <c r="D6" s="146"/>
       <c r="E6" s="69" t="s">
         <v>56</v>
       </c>
@@ -2870,15 +2894,15 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="85">
         <v>3</v>
       </c>
-      <c r="B7" s="148" t="s">
+      <c r="B7" s="144" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="149"/>
-      <c r="D7" s="150"/>
+      <c r="C7" s="145"/>
+      <c r="D7" s="146"/>
       <c r="E7" s="79" t="str">
         <f>E4</f>
         <v>1 -  11</v>
@@ -2905,15 +2929,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="85">
         <v>4</v>
       </c>
-      <c r="B8" s="151" t="s">
+      <c r="B8" s="147" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="152"/>
-      <c r="D8" s="153"/>
+      <c r="C8" s="148"/>
+      <c r="D8" s="149"/>
       <c r="E8" s="87">
         <v>2</v>
       </c>
@@ -2939,14 +2963,14 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="85">
         <v>5</v>
       </c>
       <c r="B9" s="158" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="142" t="s">
+      <c r="C9" s="150" t="s">
         <v>63</v>
       </c>
       <c r="D9" s="52" t="s">
@@ -2977,12 +3001,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="46">
         <v>6</v>
       </c>
       <c r="B10" s="159"/>
-      <c r="C10" s="143"/>
+      <c r="C10" s="151"/>
       <c r="D10" s="82" t="s">
         <v>62</v>
       </c>
@@ -3019,12 +3043,12 @@
         <v>7020</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="86">
         <v>7</v>
       </c>
       <c r="B11" s="159"/>
-      <c r="C11" s="154" t="s">
+      <c r="C11" s="152" t="s">
         <v>64</v>
       </c>
       <c r="D11" s="82" t="s">
@@ -3055,12 +3079,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="86">
         <v>8</v>
       </c>
       <c r="B12" s="159"/>
-      <c r="C12" s="155"/>
+      <c r="C12" s="153"/>
       <c r="D12" s="52" t="s">
         <v>66</v>
       </c>
@@ -3097,12 +3121,12 @@
         <v>7590</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="86">
         <v>9</v>
       </c>
       <c r="B13" s="159"/>
-      <c r="C13" s="128" t="s">
+      <c r="C13" s="154" t="s">
         <v>67</v>
       </c>
       <c r="D13" s="82" t="s">
@@ -3133,12 +3157,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="86">
         <v>10</v>
       </c>
       <c r="B14" s="160"/>
-      <c r="C14" s="129"/>
+      <c r="C14" s="155"/>
       <c r="D14" s="121" t="s">
         <v>73</v>
       </c>
@@ -3173,11 +3197,11 @@
         <v>82390</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="86">
         <v>11</v>
       </c>
-      <c r="B15" s="144" t="s">
+      <c r="B15" s="139" t="s">
         <v>75</v>
       </c>
       <c r="C15" s="161" t="s">
@@ -3212,12 +3236,12 @@
       </c>
       <c r="Q15" s="11"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="46">
         <v>12</v>
       </c>
-      <c r="B16" s="145"/>
-      <c r="C16" s="155"/>
+      <c r="B16" s="140"/>
+      <c r="C16" s="153"/>
       <c r="D16" s="82" t="s">
         <v>77</v>
       </c>
@@ -3248,11 +3272,11 @@
         <v>34051</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="86">
         <v>13</v>
       </c>
-      <c r="B17" s="145"/>
+      <c r="B17" s="140"/>
       <c r="C17" s="56" t="s">
         <v>69</v>
       </c>
@@ -3286,11 +3310,11 @@
         <v>34200</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="46">
         <v>14</v>
       </c>
-      <c r="B18" s="136"/>
+      <c r="B18" s="141"/>
       <c r="C18" s="114" t="s">
         <v>70</v>
       </c>
@@ -3326,14 +3350,14 @@
       <c r="M18" s="11"/>
       <c r="N18" s="11"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="86">
         <v>15</v>
       </c>
-      <c r="B19" s="130" t="s">
+      <c r="B19" s="167" t="s">
         <v>79</v>
       </c>
-      <c r="C19" s="142" t="s">
+      <c r="C19" s="150" t="s">
         <v>80</v>
       </c>
       <c r="D19" s="116" t="s">
@@ -3364,12 +3388,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="86">
         <v>16</v>
       </c>
-      <c r="B20" s="131"/>
-      <c r="C20" s="143"/>
+      <c r="B20" s="168"/>
+      <c r="C20" s="151"/>
       <c r="D20" s="70" t="s">
         <v>83</v>
       </c>
@@ -3407,12 +3431,12 @@
       </c>
       <c r="M20" s="7"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="85">
         <v>17</v>
       </c>
-      <c r="B21" s="131"/>
-      <c r="C21" s="128" t="s">
+      <c r="B21" s="168"/>
+      <c r="C21" s="154" t="s">
         <v>81</v>
       </c>
       <c r="D21" s="52" t="s">
@@ -3443,12 +3467,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="85">
         <v>18</v>
       </c>
-      <c r="B22" s="132"/>
-      <c r="C22" s="129"/>
+      <c r="B22" s="169"/>
+      <c r="C22" s="155"/>
       <c r="D22" s="115" t="s">
         <v>85</v>
       </c>
@@ -3484,15 +3508,15 @@
         <v>3280</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="85">
         <v>19</v>
       </c>
-      <c r="B23" s="133" t="s">
+      <c r="B23" s="170" t="s">
         <v>103</v>
       </c>
-      <c r="C23" s="134"/>
-      <c r="D23" s="135"/>
+      <c r="C23" s="171"/>
+      <c r="D23" s="172"/>
       <c r="E23" s="118">
         <f>ROUND((E10+E12+E14+E20+E22)/'4-ОМК'!H7, 2)</f>
         <v>3913.64</v>
@@ -3520,21 +3544,21 @@
       <c r="K23" s="117" t="s">
         <v>56</v>
       </c>
-      <c r="L23" s="126">
+      <c r="L23" s="165">
         <f>SUM(E24:J24)+K25</f>
         <v>232117</v>
       </c>
       <c r="S23" s="11"/>
     </row>
-    <row r="24" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="46">
         <v>20</v>
       </c>
-      <c r="B24" s="136" t="s">
+      <c r="B24" s="141" t="s">
         <v>89</v>
       </c>
-      <c r="C24" s="137"/>
-      <c r="D24" s="138"/>
+      <c r="C24" s="173"/>
+      <c r="D24" s="174"/>
       <c r="E24" s="62">
         <f>E10+E12+E14+E20+E22</f>
         <v>43050</v>
@@ -3562,52 +3586,52 @@
       <c r="K24" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="L24" s="127"/>
-    </row>
-    <row r="25" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L24" s="166"/>
+    </row>
+    <row r="25" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="86">
         <v>21</v>
       </c>
-      <c r="B25" s="139" t="s">
+      <c r="B25" s="175" t="s">
         <v>91</v>
       </c>
-      <c r="C25" s="140"/>
-      <c r="D25" s="140"/>
-      <c r="E25" s="140"/>
-      <c r="F25" s="140"/>
-      <c r="G25" s="140"/>
-      <c r="H25" s="140"/>
-      <c r="I25" s="140"/>
-      <c r="J25" s="141"/>
+      <c r="C25" s="176"/>
+      <c r="D25" s="176"/>
+      <c r="E25" s="176"/>
+      <c r="F25" s="176"/>
+      <c r="G25" s="176"/>
+      <c r="H25" s="176"/>
+      <c r="I25" s="176"/>
+      <c r="J25" s="177"/>
       <c r="K25" s="59">
         <f>K20+K12+K10+SUM(K16:K18)</f>
         <v>95279</v>
       </c>
-      <c r="L25" s="127"/>
-    </row>
-    <row r="26" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L25" s="166"/>
+    </row>
+    <row r="26" spans="1:19" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="47">
         <v>22</v>
       </c>
-      <c r="B26" s="123" t="s">
+      <c r="B26" s="162" t="s">
         <v>90</v>
       </c>
-      <c r="C26" s="124"/>
-      <c r="D26" s="124"/>
-      <c r="E26" s="124"/>
-      <c r="F26" s="124"/>
-      <c r="G26" s="124"/>
-      <c r="H26" s="124"/>
-      <c r="I26" s="124"/>
-      <c r="J26" s="124"/>
-      <c r="K26" s="124"/>
+      <c r="C26" s="163"/>
+      <c r="D26" s="163"/>
+      <c r="E26" s="163"/>
+      <c r="F26" s="163"/>
+      <c r="G26" s="163"/>
+      <c r="H26" s="163"/>
+      <c r="I26" s="163"/>
+      <c r="J26" s="163"/>
+      <c r="K26" s="163"/>
       <c r="L26" s="83">
         <f>L10+L12+L14+SUM(L16:L18)+L20+L22</f>
         <v>232117</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="K28" t="s">
         <v>95</v>
       </c>
@@ -3617,44 +3641,44 @@
       </c>
       <c r="M28" s="48"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B30" s="125" t="s">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B30" s="164" t="s">
         <v>92</v>
       </c>
-      <c r="C30" s="125"/>
+      <c r="C30" s="164"/>
       <c r="D30" s="14" t="s">
         <v>93</v>
       </c>
       <c r="E30" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="F30" s="125" t="s">
+      <c r="F30" s="164" t="s">
         <v>118</v>
       </c>
-      <c r="G30" s="125"/>
-      <c r="H30" s="125"/>
-      <c r="I30" s="125"/>
-      <c r="J30" s="125"/>
-      <c r="K30" s="125"/>
-      <c r="L30" s="125"/>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G30" s="164"/>
+      <c r="H30" s="164"/>
+      <c r="I30" s="164"/>
+      <c r="J30" s="164"/>
+      <c r="K30" s="164"/>
+      <c r="L30" s="164"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B31" s="38"/>
       <c r="C31" s="38"/>
       <c r="D31" s="38"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B32" s="38"/>
       <c r="C32" s="38"/>
       <c r="D32" s="38"/>
       <c r="J32" s="11"/>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B33" s="38"/>
       <c r="C33" s="38"/>
       <c r="D33" s="38"/>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B34" s="45"/>
       <c r="C34" s="45"/>
       <c r="D34" s="45"/>
@@ -3662,11 +3686,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="K1:K3"/>
-    <mergeCell ref="L1:L3"/>
-    <mergeCell ref="E1:J1"/>
-    <mergeCell ref="E3:J3"/>
-    <mergeCell ref="B1:D4"/>
+    <mergeCell ref="B26:K26"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="F30:L30"/>
+    <mergeCell ref="L23:L25"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:J25"/>
+    <mergeCell ref="C19:C20"/>
     <mergeCell ref="B15:B18"/>
     <mergeCell ref="A1:A4"/>
     <mergeCell ref="B6:D6"/>
@@ -3678,16 +3707,11 @@
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B9:B14"/>
     <mergeCell ref="C15:C16"/>
-    <mergeCell ref="B26:K26"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="F30:L30"/>
-    <mergeCell ref="L23:L25"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:J25"/>
-    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="K1:K3"/>
+    <mergeCell ref="L1:L3"/>
+    <mergeCell ref="E1:J1"/>
+    <mergeCell ref="E3:J3"/>
+    <mergeCell ref="B1:D4"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3695,48 +3719,48 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" customWidth="1"/>
-    <col min="14" max="14" width="14.85546875" customWidth="1"/>
-    <col min="15" max="15" width="17.28515625" customWidth="1"/>
-    <col min="17" max="17" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" customWidth="1"/>
+    <col min="3" max="3" width="6.109375" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" customWidth="1"/>
+    <col min="14" max="14" width="14.88671875" customWidth="1"/>
+    <col min="15" max="15" width="17.33203125" customWidth="1"/>
+    <col min="17" max="17" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13"/>
-      <c r="B1" s="137" t="s">
+      <c r="B1" s="173" t="s">
         <v>119</v>
       </c>
-      <c r="C1" s="137"/>
-      <c r="D1" s="137"/>
-      <c r="E1" s="137"/>
-      <c r="F1" s="137"/>
-      <c r="G1" s="137"/>
+      <c r="C1" s="173"/>
+      <c r="D1" s="173"/>
+      <c r="E1" s="173"/>
+      <c r="F1" s="173"/>
+      <c r="G1" s="173"/>
       <c r="H1" s="13"/>
-      <c r="I1" s="137" t="s">
+      <c r="I1" s="173" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="137"/>
-      <c r="K1" s="137"/>
-      <c r="L1" s="137"/>
-      <c r="M1" s="137"/>
-      <c r="N1" s="137"/>
-      <c r="O1" s="137"/>
-      <c r="P1" s="137"/>
-      <c r="Q1" s="137"/>
-      <c r="R1" s="137"/>
+      <c r="J1" s="173"/>
+      <c r="K1" s="173"/>
+      <c r="L1" s="173"/>
+      <c r="M1" s="173"/>
+      <c r="N1" s="173"/>
+      <c r="O1" s="173"/>
+      <c r="P1" s="173"/>
+      <c r="Q1" s="173"/>
+      <c r="R1" s="173"/>
       <c r="T1" s="178" t="s">
         <v>120</v>
       </c>
@@ -3748,7 +3772,7 @@
       <c r="Z1" s="178"/>
       <c r="AA1" s="178"/>
     </row>
-    <row r="2" spans="1:27" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="4">
         <v>1</v>
       </c>
@@ -3822,7 +3846,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="5">
         <v>2</v>
       </c>
@@ -3866,7 +3890,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="T4" s="5">
         <v>3</v>
       </c>
@@ -3903,26 +3927,26 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.85546875" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="35.88671875" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" customWidth="1"/>
+    <col min="9" max="9" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -3945,18 +3969,18 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B4">
         <f>SUM(H7:H11) + SUM(K7:K11) + 1</f>
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G5" t="s">
         <v>23</v>
       </c>
@@ -3964,8 +3988,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G7" t="s">
         <v>24</v>
       </c>
@@ -3987,7 +4011,7 @@
         <v>43 - 45</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G8" t="s">
         <v>25</v>
       </c>
@@ -3999,7 +4023,7 @@
         <v>12 - 18</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G9" t="s">
         <v>26</v>
       </c>
@@ -4011,7 +4035,7 @@
         <v>19 - 26</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G10" t="s">
         <v>27</v>
       </c>
@@ -4023,7 +4047,7 @@
         <v>27 - 34</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G11" t="s">
         <v>28</v>
       </c>
@@ -4035,31 +4059,31 @@
         <v>35 - 42</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="14.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="14.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="24" t="s">
         <v>20</v>
       </c>
@@ -4080,7 +4104,7 @@
       </c>
       <c r="G1" s="7"/>
     </row>
-    <row r="2" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="181" t="s">
         <v>5</v>
       </c>
@@ -4105,7 +4129,7 @@
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="182"/>
       <c r="B3" s="30" t="s">
         <v>1</v>
@@ -4128,7 +4152,7 @@
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
     </row>
-    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="182"/>
       <c r="B4" s="30" t="s">
         <v>2</v>
@@ -4151,7 +4175,7 @@
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="182"/>
       <c r="B5" s="9" t="s">
         <v>3</v>
@@ -4174,7 +4198,7 @@
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="183"/>
       <c r="B6" s="33" t="s">
         <v>4</v>
@@ -4197,7 +4221,7 @@
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="179" t="s">
         <v>10</v>
       </c>
@@ -4213,7 +4237,7 @@
       <c r="H7" s="7"/>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="181" t="s">
         <v>6</v>
       </c>
@@ -4238,7 +4262,7 @@
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
     </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="182"/>
       <c r="B9" s="26" t="s">
         <v>1</v>
@@ -4261,7 +4285,7 @@
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
     </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="182"/>
       <c r="B10" s="26" t="s">
         <v>2</v>
@@ -4285,7 +4309,7 @@
       <c r="J10" s="10"/>
       <c r="K10" s="7"/>
     </row>
-    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="182"/>
       <c r="B11" s="26" t="s">
         <v>3</v>
@@ -4309,7 +4333,7 @@
       <c r="J11" s="10"/>
       <c r="K11" s="7"/>
     </row>
-    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="183"/>
       <c r="B12" s="33" t="s">
         <v>4</v>
@@ -4332,7 +4356,7 @@
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
     </row>
-    <row r="13" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="179" t="s">
         <v>11</v>
       </c>
@@ -4345,7 +4369,7 @@
         <v>8177</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="181" t="s">
         <v>7</v>
       </c>
@@ -4370,7 +4394,7 @@
       <c r="I14" s="10"/>
       <c r="J14" s="10"/>
     </row>
-    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="182"/>
       <c r="B15" s="30" t="s">
         <v>1</v>
@@ -4393,7 +4417,7 @@
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
     </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="182"/>
       <c r="B16" s="9" t="s">
         <v>2</v>
@@ -4416,7 +4440,7 @@
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
     </row>
-    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="182"/>
       <c r="B17" s="26" t="s">
         <v>3</v>
@@ -4439,7 +4463,7 @@
       <c r="I17" s="10"/>
       <c r="J17" s="10"/>
     </row>
-    <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="183"/>
       <c r="B18" s="9" t="s">
         <v>4</v>
@@ -4463,7 +4487,7 @@
       <c r="J18" s="10"/>
       <c r="K18" s="7"/>
     </row>
-    <row r="19" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="179" t="s">
         <v>12</v>
       </c>
@@ -4480,7 +4504,7 @@
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
     </row>
-    <row r="20" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="181" t="s">
         <v>8</v>
       </c>
@@ -4502,7 +4526,7 @@
       </c>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="182"/>
       <c r="B21" s="30" t="s">
         <v>1</v>
@@ -4522,7 +4546,7 @@
       </c>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="182"/>
       <c r="B22" s="9" t="s">
         <v>2</v>
@@ -4543,7 +4567,7 @@
       <c r="G22" s="8"/>
       <c r="H22" s="7"/>
     </row>
-    <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="182"/>
       <c r="B23" s="26" t="s">
         <v>3</v>
@@ -4563,7 +4587,7 @@
       </c>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="183"/>
       <c r="B24" s="9" t="s">
         <v>4</v>
@@ -4584,7 +4608,7 @@
       <c r="G24" s="8"/>
       <c r="H24" s="7"/>
     </row>
-    <row r="25" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="179" t="s">
         <v>13</v>
       </c>
@@ -4598,7 +4622,7 @@
       </c>
       <c r="G25" s="7"/>
     </row>
-    <row r="26" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="181" t="s">
         <v>9</v>
       </c>
@@ -4621,7 +4645,7 @@
       <c r="G26" s="8"/>
       <c r="M26" s="11"/>
     </row>
-    <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="182"/>
       <c r="B27" s="26" t="s">
         <v>1</v>
@@ -4641,7 +4665,7 @@
       </c>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="182"/>
       <c r="B28" s="26" t="s">
         <v>2</v>
@@ -4661,7 +4685,7 @@
       </c>
       <c r="G28" s="8"/>
     </row>
-    <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="182"/>
       <c r="B29" s="26" t="s">
         <v>3</v>
@@ -4681,7 +4705,7 @@
       </c>
       <c r="G29" s="8"/>
     </row>
-    <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="183"/>
       <c r="B30" s="9" t="s">
         <v>4</v>
@@ -4701,7 +4725,7 @@
       </c>
       <c r="G30" s="8"/>
     </row>
-    <row r="31" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="179" t="s">
         <v>14</v>
       </c>
@@ -4715,7 +4739,7 @@
       </c>
       <c r="G31" s="7"/>
     </row>
-    <row r="32" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A31:E31"/>
@@ -4734,22 +4758,22 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L15"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="28.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B2" s="39" t="s">
         <v>39</v>
       </c>
@@ -4789,7 +4813,7 @@
         <v>34051</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E4" t="s">
         <v>42</v>
       </c>
@@ -4803,7 +4827,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C5" s="38"/>
       <c r="D5" s="38"/>
       <c r="E5" s="1">
@@ -4819,7 +4843,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" s="39" t="s">
         <v>41</v>
       </c>
@@ -4843,7 +4867,7 @@
         <v>34200</v>
       </c>
     </row>
-    <row r="9" spans="2:12" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:12" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C9" s="38"/>
       <c r="D9" s="35" t="s">
         <v>51</v>
@@ -4865,7 +4889,7 @@
       </c>
       <c r="K9" s="35"/>
     </row>
-    <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D10">
         <f>PRODUCT(H10:J10)</f>
         <v>13680</v>
@@ -4887,11 +4911,11 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C11" s="38"/>
       <c r="D11" s="38"/>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" s="39" t="s">
         <v>50</v>
       </c>
@@ -4915,7 +4939,7 @@
         <v>25300.000000000004</v>
       </c>
     </row>
-    <row r="14" spans="2:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:12" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C14" s="38"/>
       <c r="D14" s="35" t="s">
         <v>51</v>
@@ -4936,7 +4960,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D15">
         <f>PRODUCT(H15:J15)</f>
         <v>10120.000000000002</v>

</xml_diff>